<commit_message>
exercise eda score and time plots
</commit_message>
<xml_diff>
--- a/data/original/exercises/rubric.xlsx
+++ b/data/original/exercises/rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie\git\hub\dissertation\submodules\dissertation-analysis\data\original\exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4DCF0A-2470-43DC-B76B-D93066193677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DF3166-9F00-4C57-B013-3FEFD07BCED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="9570" windowWidth="10890" windowHeight="11325" xr2:uid="{F1DFA896-92EB-49F6-AA66-C32F946EC712}"/>
+    <workbookView xWindow="30075" yWindow="1380" windowWidth="14565" windowHeight="18240" xr2:uid="{F1DFA896-92EB-49F6-AA66-C32F946EC712}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>pre</t>
   </si>
@@ -92,6 +92,9 @@
 for groupby
 for summarize
 mean (na.rm = TRUE) or used dropna</t>
+  </si>
+  <si>
+    <t>rubric</t>
   </si>
 </sst>
 </file>
@@ -448,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC38FD48-D90D-482F-89CA-0DBAD355C630}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,6 +467,9 @@
       <c r="B1" t="s">
         <v>6</v>
       </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>